<commit_message>
WordPress user login with selenium automation
</commit_message>
<xml_diff>
--- a/WordPress-version-6-1-1/user-login/Test Cases WordPress Users.xlsx
+++ b/WordPress-version-6-1-1/user-login/Test Cases WordPress Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Lacie\My Documents plus Web Design\websites\ggeorgiou.work\testing-wordpress\WordPress-version-6-1-1\user-login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965F5F31-D1A7-4F42-9EB5-BFE5162DBD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03823ECC-B198-4953-8958-6B5D0A4B9F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="255" windowWidth="24825" windowHeight="11475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14865" yWindow="2265" windowWidth="22470" windowHeight="12945" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -666,295 +666,7 @@
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="141">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="105">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2180,7 +1892,7 @@
   <dimension ref="B1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2475,7 +2187,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2772,7 +2484,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>84</v>
@@ -3390,332 +3102,332 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="F4:G5 F8:G9 F12:G13 F16:G17 F20:G21 F24:G25">
-    <cfRule type="containsText" dxfId="53" priority="127" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="104" priority="127" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:G5 F8:G9 F12:G13 F16:G17 F20:G21 F24:G25">
-    <cfRule type="containsText" dxfId="52" priority="128" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="103" priority="128" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:G5 F8:G9 F12:G13 F16:G17 F20:G21 F24:G25">
-    <cfRule type="containsText" dxfId="51" priority="129" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="102" priority="129" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:G29">
-    <cfRule type="containsText" dxfId="140" priority="124" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="101" priority="124" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:G29">
-    <cfRule type="containsText" dxfId="139" priority="125" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="100" priority="125" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:G29">
-    <cfRule type="containsText" dxfId="138" priority="126" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="99" priority="126" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:G33">
-    <cfRule type="containsText" dxfId="137" priority="121" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="98" priority="121" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:G33">
-    <cfRule type="containsText" dxfId="136" priority="122" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="97" priority="122" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:G33">
-    <cfRule type="containsText" dxfId="135" priority="123" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="96" priority="123" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:G37">
-    <cfRule type="containsText" dxfId="134" priority="118" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="95" priority="118" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F36))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:G37">
-    <cfRule type="containsText" dxfId="133" priority="119" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="94" priority="119" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F36))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:G37">
-    <cfRule type="containsText" dxfId="132" priority="120" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="93" priority="120" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F36))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40:G41">
-    <cfRule type="containsText" dxfId="131" priority="115" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="92" priority="115" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40:G41">
-    <cfRule type="containsText" dxfId="130" priority="116" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="91" priority="116" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40:G41">
-    <cfRule type="containsText" dxfId="129" priority="117" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="90" priority="117" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:G45">
-    <cfRule type="containsText" dxfId="128" priority="112" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="89" priority="112" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F44))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:G45">
-    <cfRule type="containsText" dxfId="127" priority="113" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="88" priority="113" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F44))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:G45">
-    <cfRule type="containsText" dxfId="126" priority="114" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="87" priority="114" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F44))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:G49">
-    <cfRule type="containsText" dxfId="125" priority="109" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="86" priority="109" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F48))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:G49">
-    <cfRule type="containsText" dxfId="124" priority="110" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="85" priority="110" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F48))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:G49">
-    <cfRule type="containsText" dxfId="123" priority="111" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="84" priority="111" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F48))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G53">
-    <cfRule type="containsText" dxfId="122" priority="106" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="83" priority="106" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F52))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G53">
-    <cfRule type="containsText" dxfId="121" priority="107" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="82" priority="107" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F52))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G53">
-    <cfRule type="containsText" dxfId="120" priority="108" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="81" priority="108" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F52))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:G57 F58">
-    <cfRule type="containsText" dxfId="119" priority="103" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="80" priority="103" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F56))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:G57 F58">
-    <cfRule type="containsText" dxfId="118" priority="104" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="79" priority="104" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F56))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:G57 F58">
-    <cfRule type="containsText" dxfId="117" priority="105" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="78" priority="105" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F56))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="containsText" dxfId="92" priority="76" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F54))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="containsText" dxfId="91" priority="77" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F54))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="containsText" dxfId="90" priority="78" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F54))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="89" priority="73" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F50))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="88" priority="74" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F50))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="87" priority="75" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F50))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="containsText" dxfId="86" priority="70" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F46))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="containsText" dxfId="85" priority="71" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F46))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="containsText" dxfId="84" priority="72" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F46))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="83" priority="67" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F42))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="82" priority="68" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F42))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="81" priority="69" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F42))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="containsText" dxfId="80" priority="64" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F38))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="containsText" dxfId="79" priority="65" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F38))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="containsText" dxfId="78" priority="66" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F38))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="containsText" dxfId="77" priority="61" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="containsText" dxfId="76" priority="62" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="containsText" dxfId="75" priority="63" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsText" dxfId="74" priority="58" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsText" dxfId="73" priority="59" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsText" dxfId="72" priority="60" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="containsText" dxfId="71" priority="55" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F26))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="containsText" dxfId="70" priority="56" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F26))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="containsText" dxfId="69" priority="57" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F26))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="68" priority="52" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F22))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="67" priority="53" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F22))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="66" priority="54" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F22))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsText" dxfId="65" priority="49" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsText" dxfId="64" priority="50" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsText" dxfId="63" priority="51" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="62" priority="46" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="61" priority="47" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="60" priority="48" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="59" priority="43" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="58" priority="44" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="57" priority="45" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6">
-    <cfRule type="containsText" dxfId="56" priority="40" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(F6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6">
-    <cfRule type="containsText" dxfId="55" priority="41" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(F6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6">
-    <cfRule type="containsText" dxfId="54" priority="42" operator="containsText" text="Block / Skip">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(F6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3923,5 +3635,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>